<commit_message>
add 7inch Front-panel layout
</commit_message>
<xml_diff>
--- a/Scheme/Front-Panel.xlsx
+++ b/Scheme/Front-Panel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Develop\Projects\WOLF\Scheme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$Q$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$Q$21</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>MODE+</t>
   </si>
@@ -124,13 +124,67 @@
   </si>
   <si>
     <t>SERVICES</t>
+  </si>
+  <si>
+    <t>FRONT-3'2</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>A/B
+A=B</t>
+  </si>
+  <si>
+    <t>MODE+
+MODE-</t>
+  </si>
+  <si>
+    <t>BAND+
+BAND-</t>
+  </si>
+  <si>
+    <t>TANGENT</t>
+  </si>
+  <si>
+    <t>AUDIO 1</t>
+  </si>
+  <si>
+    <t>AUDIO 2</t>
+  </si>
+  <si>
+    <t>AUDIO 3</t>
+  </si>
+  <si>
+    <t>FRONT-7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +202,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -275,11 +339,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +462,57 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -643,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Z16"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,18 +810,23 @@
     <col min="25" max="26" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D1" s="29"/>
+    </row>
     <row r="2" spans="1:26" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="5" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="22"/>
+      <c r="G3" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="39"/>
       <c r="N3" s="19" t="s">
         <v>17</v>
       </c>
@@ -690,20 +847,20 @@
       <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="25"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="25"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="42"/>
       <c r="N5" s="9"/>
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
@@ -721,12 +878,12 @@
       <c r="E6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="25"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="42"/>
       <c r="N6" s="13"/>
       <c r="O6" s="14" t="s">
         <v>2</v>
@@ -734,12 +891,12 @@
       <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:26" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="28"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="45"/>
       <c r="N7" s="16"/>
       <c r="O7" s="17"/>
       <c r="P7" s="18"/>
@@ -793,25 +950,119 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
+    <row r="10" spans="1:26" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="32"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="24"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:26" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="24"/>
+      <c r="Q16" s="5"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
@@ -822,9 +1073,127 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="G3:L7"/>
+    <mergeCell ref="D13:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="45" orientation="portrait" r:id="rId1"/>

</xml_diff>